<commit_message>
change paramter names msa compare workflow
</commit_message>
<xml_diff>
--- a/docker/dev_elixir/workflows/msa_group_compare.cwl.job_templ.xlsx
+++ b/docker/dev_elixir/workflows/msa_group_compare.cwl.job_templ.xlsx
@@ -73,32 +73,56 @@
     <t>parameter_sheet_name</t>
   </si>
   <si>
-    <t>color_by_group</t>
-  </si>
-  <si>
-    <t>boolean</t>
+    <t>fasta_1</t>
+  </si>
+  <si>
+    <t>File</t>
   </si>
   <si>
     <t>False</t>
   </si>
   <si>
+    <t xml:space="preserve">Protein / DNA / RNA sequences of first group in fasta format.
+</t>
+  </si>
+  <si>
+    <t>parameters</t>
+  </si>
+  <si>
+    <t>fasta_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protein / DNA / RNA sequences of second group in fasta format.
+</t>
+  </si>
+  <si>
+    <t>group_name_1</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
     <t>True</t>
   </si>
   <si>
-    <t>'True'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whether to color the phylogenetic tree by group.
+    <t>'group1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of first group.
 </t>
   </si>
   <si>
-    <t>parameters</t>
-  </si>
-  <si>
-    <t>distance_method</t>
-  </si>
-  <si>
-    <t>string</t>
+    <t>group_name_2</t>
+  </si>
+  <si>
+    <t>'group2'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of second group.
+</t>
+  </si>
+  <si>
+    <t>homology_method</t>
   </si>
   <si>
     <t>'identity'</t>
@@ -109,43 +133,6 @@
   </si>
   <si>
     <t>'identity' | 'similarity'</t>
-  </si>
-  <si>
-    <t>fasta_1</t>
-  </si>
-  <si>
-    <t>File</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protein / DNA / RNA sequences of first group in fasta format.
-</t>
-  </si>
-  <si>
-    <t>fasta_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protein / DNA / RNA sequences of second group in fasta format.
-</t>
-  </si>
-  <si>
-    <t>group_name_1</t>
-  </si>
-  <si>
-    <t>'group1'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of first group.
-</t>
-  </si>
-  <si>
-    <t>group_name_2</t>
-  </si>
-  <si>
-    <t>'group2'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of second group.
-</t>
   </si>
   <si>
     <t>msa_method</t>
@@ -176,25 +163,38 @@
     <t>'protein' | 'dna' | 'rna'</t>
   </si>
   <si>
+    <t>tree_color_by_group</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>'True'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether to color the phylogenetic tree by group.
+</t>
+  </si>
+  <si>
     <t># type: param| format: vertical</t>
   </si>
   <si>
+    <t>protein</t>
+  </si>
+  <si>
+    <t>Please fill</t>
+  </si>
+  <si>
+    <t>identity</t>
+  </si>
+  <si>
+    <t>group1</t>
+  </si>
+  <si>
+    <t>group2</t>
+  </si>
+  <si>
     <t>ClustalW</t>
-  </si>
-  <si>
-    <t>group1</t>
-  </si>
-  <si>
-    <t>protein</t>
-  </si>
-  <si>
-    <t>Please fill</t>
-  </si>
-  <si>
-    <t>identity</t>
-  </si>
-  <si>
-    <t>group2</t>
   </si>
   <si>
     <t># type: metadata</t>
@@ -218,7 +218,7 @@
     <t>workflow_path</t>
   </si>
   <si>
-    <t>/mnt/c/Users/kerst/OneDrive/home/cwlab_testing/scratch/temp/UGIpYkfJbXSRax/packed.cwl</t>
+    <t>/mnt/c/Users/kerst/OneDrive/home/cwlab_testing/scratch/temp/f2phd33aq5XHyh/packed.cwl</t>
   </si>
   <si>
     <t>workflow_type</t>
@@ -652,17 +652,15 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s"/>
+      <c r="G3" t="s"/>
+      <c r="H3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s"/>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
       </c>
       <c r="I3" t="s"/>
       <c r="J3" t="s"/>
@@ -673,66 +671,64 @@
       <c r="O3" t="s"/>
       <c r="P3" t="s"/>
       <c r="Q3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s"/>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
+      <c r="G4" t="s"/>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s"/>
       <c r="J4" t="s"/>
       <c r="K4" t="s"/>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
+      <c r="L4" t="s"/>
       <c r="M4" t="s"/>
       <c r="N4" t="s"/>
       <c r="O4" t="s"/>
       <c r="P4" t="s"/>
       <c r="Q4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5" t="s"/>
-      <c r="G5" t="s"/>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s"/>
       <c r="J5" t="s"/>
@@ -743,29 +739,31 @@
       <c r="O5" t="s"/>
       <c r="P5" t="s"/>
       <c r="Q5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s"/>
+      <c r="G6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s"/>
-      <c r="G6" t="s"/>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s"/>
       <c r="J6" t="s"/>
@@ -776,12 +774,12 @@
       <c r="O6" t="s"/>
       <c r="P6" t="s"/>
       <c r="Q6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -790,33 +788,35 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
       </c>
       <c r="F7" t="s"/>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s"/>
       <c r="J7" t="s"/>
       <c r="K7" t="s"/>
-      <c r="L7" t="s"/>
+      <c r="L7" t="s">
+        <v>36</v>
+      </c>
       <c r="M7" t="s"/>
       <c r="N7" t="s"/>
       <c r="O7" t="s"/>
       <c r="P7" t="s"/>
       <c r="Q7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
@@ -825,28 +825,30 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
       <c r="F8" t="s"/>
       <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
         <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>40</v>
       </c>
       <c r="I8" t="s"/>
       <c r="J8" t="s"/>
       <c r="K8" t="s"/>
-      <c r="L8" t="s"/>
+      <c r="L8" t="s">
+        <v>40</v>
+      </c>
       <c r="M8" t="s"/>
       <c r="N8" t="s"/>
       <c r="O8" t="s"/>
       <c r="P8" t="s"/>
       <c r="Q8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -860,7 +862,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -883,7 +885,7 @@
       <c r="O9" t="s"/>
       <c r="P9" t="s"/>
       <c r="Q9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
@@ -891,36 +893,34 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
       <c r="F10" t="s"/>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s"/>
       <c r="J10" t="s"/>
       <c r="K10" t="s"/>
-      <c r="L10" t="s">
-        <v>48</v>
-      </c>
+      <c r="L10" t="s"/>
       <c r="M10" t="s"/>
       <c r="N10" t="s"/>
       <c r="O10" t="s"/>
       <c r="P10" t="s"/>
       <c r="Q10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -956,7 +956,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -967,36 +967,36 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>55</v>

</xml_diff>